<commit_message>
audit testing to xlsm
</commit_message>
<xml_diff>
--- a/Dynamic Sudit List Tests.xlsx
+++ b/Dynamic Sudit List Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scorpio\Documents\GitHub\excel-at-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25EFA013-0460-448A-8FD5-3BE0031FDF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DF39A8-D86C-481A-9F33-4935E5AAF237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{2132B190-7200-4F6F-AFEF-2049BD8F2BB1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -607,7 +607,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="m/d/yyyy\ h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -653,9 +653,9 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -703,16 +703,16 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="m/d/yyyy\ h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -731,6 +731,73 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>495300</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="CommandButton1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -768,15 +835,15 @@
     <sortCondition ref="I1:I16"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{F1031C91-AF2B-406A-8FB0-CABF1DD7AC88}" name="Manager" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{F1031C91-AF2B-406A-8FB0-CABF1DD7AC88}" name="Manager" dataDxfId="11">
       <calculatedColumnFormula>_xlfn.XLOOKUP(rot_db[[#This Row],[Name]],tm_db[Default Name],tm_db[Manager],_xlfn.XLOOKUP(rot_db[[#This Row],[Name]],tm_db[Modified Name],tm_db[Manager], "NOT IN DB", 0, 1), 0, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{07E50BFD-3A1F-47C9-89FF-5A4B1310CF9F}" name="Unified Name" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{07E50BFD-3A1F-47C9-89FF-5A4B1310CF9F}" name="Unified Name" dataDxfId="10">
       <calculatedColumnFormula>_xlfn.XLOOKUP(rot_db[[#This Row],[Name]], tm_db[Modified Name], tm_db[Device Tracker Name], "DEFAULT NAME", 0, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{FE817EF8-6303-4B8F-9B20-E3FBBEEDAAEB}" name="Name"/>
     <tableColumn id="2" xr3:uid="{725AE6B2-7BC2-43AC-A4F5-0F932374C618}" name="Position"/>
-    <tableColumn id="3" xr3:uid="{0284F5FD-6005-4336-A7D7-35C530E752A8}" name="Area" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{0284F5FD-6005-4336-A7D7-35C530E752A8}" name="Area" dataDxfId="9">
       <calculatedColumnFormula>_xlfn.XLOOKUP(rot_db[[#This Row],[Position]],pos_db[Position],pos_db[Area], "", 0, 1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -792,12 +859,12 @@
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C70A1D53-904E-40F4-90F5-402E318E858A}" name="Asset Tag"/>
-    <tableColumn id="2" xr3:uid="{660081C5-85CE-4DB2-A779-648A36D148FF}" name="Serial Number" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{5CE03F51-3827-43F6-97D3-6DEE24FD9B14}" name="Device Type" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{660081C5-85CE-4DB2-A779-648A36D148FF}" name="Serial Number" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{5CE03F51-3827-43F6-97D3-6DEE24FD9B14}" name="Device Type" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{DB0F53B8-FD3A-44D0-9657-550C5F38C88D}" name="Checked Out To"/>
-    <tableColumn id="4" xr3:uid="{6607404C-4DDC-463C-9B34-AE2E6164C360}" name="Date" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{6607404C-4DDC-463C-9B34-AE2E6164C360}" name="Date" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{087FACF2-8154-41DC-81C5-91E7BAF60086}" name="Area"/>
-    <tableColumn id="7" xr3:uid="{DD29E2DF-53DE-4E05-865B-6AE1ADE4119B}" name="Device Count" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{DD29E2DF-53DE-4E05-865B-6AE1ADE4119B}" name="Device Count" dataDxfId="5">
       <calculatedColumnFormula>IF(D2 = D1, G1 + 1, 1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1122,6 +1189,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51114517-D7F4-41FC-9B62-858E495EF210}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2226,11 +2294,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C47F9E-358C-41BA-A720-2E83F2B7D5D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C47F9E-358C-41BA-A720-2E83F2B7D5D1}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,7 +2389,7 @@
         <v>166</v>
       </c>
       <c r="G2">
-        <f>IF(D2 = D1, G1 + 1, 1)</f>
+        <f t="shared" ref="G2:G41" si="0">IF(D2 = D1, G1 + 1, 1)</f>
         <v>1</v>
       </c>
       <c r="H2" s="3"/>
@@ -2381,7 +2450,7 @@
         <v>166</v>
       </c>
       <c r="G3">
-        <f>IF(D3 = D2, G2 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
@@ -2454,7 +2523,7 @@
         <v>166</v>
       </c>
       <c r="G4">
-        <f>IF(D4 = D3, G3 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4" t="str">
@@ -2511,7 +2580,7 @@
         <v>166</v>
       </c>
       <c r="G5">
-        <f>IF(D5 = D4, G4 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I5" t="str">
@@ -2568,7 +2637,7 @@
         <v>166</v>
       </c>
       <c r="G6">
-        <f>IF(D6 = D5, G5 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M6" t="str">
@@ -2579,7 +2648,7 @@
         <v>1</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O8" si="0">IF(ISNUMBER(O5), O5 + N6 + 1,1)</f>
+        <f t="shared" ref="O6:O8" si="1">IF(ISNUMBER(O5), O5 + N6 + 1,1)</f>
         <v>7</v>
       </c>
       <c r="U6" t="str">
@@ -2590,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="W6">
-        <f t="shared" ref="W6:W7" si="1">IF(ISNUMBER(W5), W5 + V6 + 1,1)</f>
+        <f t="shared" ref="W6:W7" si="2">IF(ISNUMBER(W5), W5 + V6 + 1,1)</f>
         <v>7</v>
       </c>
     </row>
@@ -2614,7 +2683,7 @@
         <v>166</v>
       </c>
       <c r="G7">
-        <f>IF(D7 = D6, G6 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M7" t="str">
@@ -2625,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="U7" t="str">
@@ -2636,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -2660,7 +2729,7 @@
         <v>166</v>
       </c>
       <c r="G8">
-        <f>IF(D8 = D7, G7 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M8" t="str">
@@ -2671,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -2695,7 +2764,7 @@
         <v>166</v>
       </c>
       <c r="G9">
-        <f>IF(D9 = D8, G8 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2719,7 +2788,7 @@
         <v>166</v>
       </c>
       <c r="G10">
-        <f>IF(D10 = D9, G9 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2743,7 +2812,7 @@
         <v>166</v>
       </c>
       <c r="G11">
-        <f>IF(D11 = D10, G10 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2767,7 +2836,7 @@
         <v>166</v>
       </c>
       <c r="G12">
-        <f>IF(D12 = D11, G11 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2791,7 +2860,7 @@
         <v>166</v>
       </c>
       <c r="G13">
-        <f>IF(D13 = D12, G12 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -2815,7 +2884,7 @@
         <v>166</v>
       </c>
       <c r="G14">
-        <f>IF(D14 = D13, G13 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -2839,7 +2908,7 @@
         <v>166</v>
       </c>
       <c r="G15">
-        <f>IF(D15 = D14, G14 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2863,7 +2932,7 @@
         <v>166</v>
       </c>
       <c r="G16">
-        <f>IF(D16 = D15, G15 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2887,7 +2956,7 @@
         <v>166</v>
       </c>
       <c r="G17">
-        <f>IF(D17 = D16, G16 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2911,7 +2980,7 @@
         <v>166</v>
       </c>
       <c r="G18">
-        <f>IF(D18 = D17, G17 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2935,7 +3004,7 @@
         <v>166</v>
       </c>
       <c r="G19">
-        <f>IF(D19 = D18, G18 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2959,7 +3028,7 @@
         <v>166</v>
       </c>
       <c r="G20">
-        <f>IF(D20 = D19, G19 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2983,7 +3052,7 @@
         <v>166</v>
       </c>
       <c r="G21">
-        <f>IF(D21 = D20, G20 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3007,7 +3076,7 @@
         <v>166</v>
       </c>
       <c r="G22">
-        <f>IF(D22 = D21, G21 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3031,7 +3100,7 @@
         <v>166</v>
       </c>
       <c r="G23">
-        <f>IF(D23 = D22, G22 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3055,7 +3124,7 @@
         <v>166</v>
       </c>
       <c r="G24">
-        <f>IF(D24 = D23, G23 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3079,7 +3148,7 @@
         <v>166</v>
       </c>
       <c r="G25">
-        <f>IF(D25 = D24, G24 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3103,7 +3172,7 @@
         <v>166</v>
       </c>
       <c r="G26">
-        <f>IF(D26 = D25, G25 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3127,7 +3196,7 @@
         <v>166</v>
       </c>
       <c r="G27">
-        <f>IF(D27 = D26, G26 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3151,7 +3220,7 @@
         <v>166</v>
       </c>
       <c r="G28">
-        <f>IF(D28 = D27, G27 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3175,7 +3244,7 @@
         <v>166</v>
       </c>
       <c r="G29">
-        <f>IF(D29 = D28, G28 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3199,7 +3268,7 @@
         <v>166</v>
       </c>
       <c r="G30">
-        <f>IF(D30 = D29, G29 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3223,7 +3292,7 @@
         <v>166</v>
       </c>
       <c r="G31">
-        <f>IF(D31 = D30, G30 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3247,7 +3316,7 @@
         <v>166</v>
       </c>
       <c r="G32">
-        <f>IF(D32 = D31, G31 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3271,7 +3340,7 @@
         <v>166</v>
       </c>
       <c r="G33">
-        <f>IF(D33 = D32, G32 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3295,7 +3364,7 @@
         <v>166</v>
       </c>
       <c r="G34">
-        <f>IF(D34 = D33, G33 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3319,7 +3388,7 @@
         <v>166</v>
       </c>
       <c r="G35">
-        <f>IF(D35 = D34, G34 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3343,7 +3412,7 @@
         <v>166</v>
       </c>
       <c r="G36">
-        <f>IF(D36 = D35, G35 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3367,7 +3436,7 @@
         <v>166</v>
       </c>
       <c r="G37">
-        <f>IF(D37 = D36, G36 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3391,7 +3460,7 @@
         <v>166</v>
       </c>
       <c r="G38">
-        <f>IF(D38 = D37, G37 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3415,7 +3484,7 @@
         <v>166</v>
       </c>
       <c r="G39">
-        <f>IF(D39 = D38, G38 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3439,7 +3508,7 @@
         <v>166</v>
       </c>
       <c r="G40">
-        <f>IF(D40 = D39, G39 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3463,7 +3532,7 @@
         <v>166</v>
       </c>
       <c r="G41">
-        <f>IF(D41 = D40, G40 + 1, 1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3484,14 +3553,44 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId3" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>495300</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>14</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId3" name="CommandButton1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1991A9C5-A1CB-4795-8A14-055598C8BB4D}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">

</xml_diff>